<commit_message>
[CHG] FINALIZAÇÃO DO MODELO PONDERADO COM VÁRIOS PESOS
</commit_message>
<xml_diff>
--- a/data/Manutencoes_Agencias.xlsx
+++ b/data/Manutencoes_Agencias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson\Desktop\Itaú\Comunidade Infra de Canais Físicos\Projetos\IBS 360\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="17">
   <si>
     <t>Agência</t>
   </si>
@@ -443,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1455,7 @@
         <v>45126</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E59" s="2">
         <v>2420</v>
@@ -1493,6 +1493,23 @@
       </c>
       <c r="E61" s="2">
         <v>627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>10</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="3">
+        <v>45129</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="2">
+        <v>3200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CHG] REESTRUTURANDO AS FUNÇOES
</commit_message>
<xml_diff>
--- a/data/Manutencoes_Agencias.xlsx
+++ b/data/Manutencoes_Agencias.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VOLUME" sheetId="1" r:id="rId1"/>
+    <sheet name="CUSTO" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="21">
   <si>
     <t>Agência</t>
   </si>
@@ -70,6 +71,18 @@
   </si>
   <si>
     <t>Não</t>
+  </si>
+  <si>
+    <t>Outlier Superior</t>
+  </si>
+  <si>
+    <t>Outlier Inferior</t>
+  </si>
+  <si>
+    <t>Custo 2</t>
+  </si>
+  <si>
+    <t>Tipo de outlier</t>
   </si>
 </sst>
 </file>
@@ -128,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -138,6 +151,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,4 +1534,502 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5867</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1339</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3045</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3293</v>
+      </c>
+      <c r="D5" s="2">
+        <v>16448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3533</v>
+      </c>
+      <c r="D6" s="2">
+        <v>11156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9656</v>
+      </c>
+      <c r="D7" s="2">
+        <v>17077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1956</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1838</v>
+      </c>
+      <c r="D9" s="2">
+        <v>16852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3448</v>
+      </c>
+      <c r="D10" s="2">
+        <v>16029</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9742</v>
+      </c>
+      <c r="D11" s="2">
+        <v>19814</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3600</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>4100</v>
+      </c>
+      <c r="D13" s="2">
+        <v>19674</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2800</v>
+      </c>
+      <c r="D14" s="2">
+        <v>19389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D15" s="2">
+        <v>18854</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>4500</v>
+      </c>
+      <c r="D16" s="2">
+        <v>19884</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3900</v>
+      </c>
+      <c r="D17" s="2">
+        <v>12652</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3300</v>
+      </c>
+      <c r="D18" s="2">
+        <v>14145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1200</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2">
+        <v>11367</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D20" s="2">
+        <v>18137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4800</v>
+      </c>
+      <c r="D21" s="2">
+        <v>16610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4600</v>
+      </c>
+      <c r="D22" s="2">
+        <v>17720</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5">
+        <v>3400</v>
+      </c>
+      <c r="D23" s="2">
+        <v>18931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5200</v>
+      </c>
+      <c r="D24" s="2">
+        <v>12939</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D25" s="2">
+        <v>15539</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4300</v>
+      </c>
+      <c r="D26" s="2">
+        <v>10869</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3700</v>
+      </c>
+      <c r="D27" s="2">
+        <v>15117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2200</v>
+      </c>
+      <c r="D28" s="2">
+        <v>18553</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>3900</v>
+      </c>
+      <c r="D29" s="2">
+        <v>17957</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4700</v>
+      </c>
+      <c r="D30" s="2">
+        <v>12385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5300</v>
+      </c>
+      <c r="D31" s="2">
+        <v>13583</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5">
+        <v>5800</v>
+      </c>
+      <c r="D32" s="2">
+        <v>14150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5">
+        <v>15000</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="2">
+        <v>10712</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5">
+        <v>3600</v>
+      </c>
+      <c r="D34" s="2">
+        <v>14897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5">
+        <v>4200</v>
+      </c>
+      <c r="D35" s="2">
+        <v>13975</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5">
+        <v>4300</v>
+      </c>
+      <c r="D36" s="2">
+        <v>11901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2900</v>
+      </c>
+      <c r="D37" s="2">
+        <v>12138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1100</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="2">
+        <v>18614</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5">
+        <v>2400</v>
+      </c>
+      <c r="D39" s="2">
+        <v>19691</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5">
+        <v>4900</v>
+      </c>
+      <c r="D40" s="2">
+        <v>19945</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5">
+        <v>16000</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="2">
+        <v>12899</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>